<commit_message>
adding thesis and results
</commit_message>
<xml_diff>
--- a/results/classification.xlsx
+++ b/results/classification.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dillorr/defaultRate/dillon/defaultRate/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7837893-7A05-CC40-9313-15D64C177961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF59C7FD-C671-D140-B86B-C6DB6E186E72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="34900" windowHeight="21940" xr2:uid="{F4DD7647-27C0-5940-9CE4-E5384D85FC8A}"/>
+    <workbookView xWindow="10740" yWindow="460" windowWidth="25100" windowHeight="21940" xr2:uid="{F4DD7647-27C0-5940-9CE4-E5384D85FC8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="21">
   <si>
     <t>Predict Proprietary School Type</t>
   </si>
@@ -77,29 +77,35 @@
     <t>Random Forest</t>
   </si>
   <si>
-    <t>Table 2</t>
-  </si>
-  <si>
-    <t>Table 1</t>
-  </si>
-  <si>
     <t>Full</t>
   </si>
   <si>
     <t>Reduced</t>
   </si>
   <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>Table 4</t>
+    <t>highWhite</t>
+  </si>
+  <si>
+    <t>Proprietary</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>All Schools</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,9 +134,16 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Var(--jp-code-font-family)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -167,11 +180,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -181,9 +204,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -495,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB15BD4-7A41-814A-9683-496F8ABF4D0F}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B51" sqref="B51:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -507,32 +541,40 @@
     <col min="2" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -551,8 +593,14 @@
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -571,8 +619,14 @@
       <c r="F4" s="2">
         <v>0.93065896979359797</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" s="2"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -591,28 +645,40 @@
       <c r="F5" s="2">
         <v>0.96620237607537895</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="10">
         <v>0.46282372598162003</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="10">
         <v>0.170752324598478</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="10">
         <v>0.175652173913043</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="10">
         <v>0.22452850968100299</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="10">
         <v>0.53304666513639098</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" s="2"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -631,8 +697,14 @@
       <c r="F7" s="2">
         <v>0.61556293749888602</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" s="10"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -652,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:13">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -672,7 +744,7 @@
         <v>0.95661827832499102</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:13">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -680,29 +752,33 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:13">
       <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
@@ -721,8 +797,26 @@
       <c r="F13" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -741,8 +835,26 @@
       <c r="F14" s="7">
         <v>0.88359296795682396</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0.95405179615705904</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0.87452471482889704</v>
+      </c>
+      <c r="K14" s="13">
+        <v>1</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0.89832109642262303</v>
+      </c>
+      <c r="M14" s="13">
+        <v>0.96620237607537895</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -761,8 +873,26 @@
       <c r="F15" s="7">
         <v>0.96620237607537895</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="H15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0.868003341687552</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0.73214285714285698</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0.92695652173913001</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0.71675220564766895</v>
+      </c>
+      <c r="M15" s="13">
+        <v>0.88359296795682396</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -781,8 +911,26 @@
       <c r="F16" s="7">
         <v>0.38688385016832</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="13">
+        <v>0.64773043720412105</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0.456603773584905</v>
+      </c>
+      <c r="K16" s="13">
+        <v>0.52608695652173898</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0.222184932943508</v>
+      </c>
+      <c r="M16" s="13">
+        <v>0.61556293749888602</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -801,8 +949,26 @@
       <c r="F17" s="7">
         <v>0.61556293749888602</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0.46282372598162003</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0.170752324598478</v>
+      </c>
+      <c r="K17" s="13">
+        <v>0.175652173913043</v>
+      </c>
+      <c r="L17" s="13">
+        <v>-0.22452850968100299</v>
+      </c>
+      <c r="M17" s="13">
+        <v>0.38688385016832</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -822,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:13">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -842,29 +1008,41 @@
         <v>0.953884010473255</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
-      </c>
+    <row r="20" spans="1:13">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
         <v>1</v>
       </c>
@@ -883,8 +1061,14 @@
       <c r="F23" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -903,8 +1087,14 @@
       <c r="F24" s="2">
         <v>0.93065896979359797</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="H24" s="2"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -923,8 +1113,14 @@
       <c r="F25" s="2">
         <v>0.88862743351798101</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="H25" s="2"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -943,8 +1139,14 @@
       <c r="F26" s="2">
         <v>0.53304666513639098</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="H26" s="2"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -958,13 +1160,19 @@
         <v>0.29677060133630201</v>
       </c>
       <c r="E27" s="2">
-        <v>0.16227127490218299</v>
+        <v>-0.16227127490218299</v>
       </c>
       <c r="F27" s="2">
         <v>0.418858838272608</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="H27" s="2"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -984,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:13">
       <c r="A29" s="4" t="s">
         <v>13</v>
       </c>
@@ -1004,29 +1212,41 @@
         <v>0.99805044946678101</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="30" spans="1:13">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:13">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="4" t="s">
         <v>1</v>
       </c>
@@ -1045,8 +1265,26 @@
       <c r="F33" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="H33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
@@ -1065,8 +1303,26 @@
       <c r="F34" s="2">
         <v>0.93065896979359797</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="H34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="13">
+        <v>0.41882483987747099</v>
+      </c>
+      <c r="J34" s="13">
+        <v>0.39277818717759699</v>
+      </c>
+      <c r="K34" s="13">
+        <v>0.29677060133630201</v>
+      </c>
+      <c r="L34" s="13">
+        <v>-0.16227127490218299</v>
+      </c>
+      <c r="M34" s="13">
+        <v>0.73501273533655098</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="2" t="s">
         <v>9</v>
       </c>
@@ -1085,8 +1341,26 @@
       <c r="F35" s="7">
         <v>0.88862743351798101</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="H35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="13">
+        <v>0.93065998329156197</v>
+      </c>
+      <c r="J35" s="13">
+        <v>0.92758430071862896</v>
+      </c>
+      <c r="K35" s="13">
+        <v>0.93429844097995496</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0.861319676215761</v>
+      </c>
+      <c r="M35" s="11">
+        <v>0.67185009707354404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="2" t="s">
         <v>10</v>
       </c>
@@ -1105,8 +1379,26 @@
       <c r="F36" s="7">
         <v>0.53304666513639098</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="H36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="13">
+        <v>0.24171539961013599</v>
+      </c>
+      <c r="J36" s="13">
+        <v>0.25227151256012798</v>
+      </c>
+      <c r="K36" s="13">
+        <v>0.262806236080178</v>
+      </c>
+      <c r="L36" s="13">
+        <v>-0.51658695957310996</v>
+      </c>
+      <c r="M36" s="13">
+        <v>0.60350373154266701</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
@@ -1125,8 +1417,26 @@
       <c r="F37" s="7">
         <v>0.418858838272608</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="H37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="13">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="J37" s="13">
+        <v>0.60006682258603405</v>
+      </c>
+      <c r="K37" s="13">
+        <v>1</v>
+      </c>
+      <c r="L37" s="13">
+        <v>0.33320949242861497</v>
+      </c>
+      <c r="M37" s="13">
+        <v>0.38775145610316503</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -1146,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:13">
       <c r="A39" s="4" t="s">
         <v>13</v>
       </c>
@@ -1166,7 +1476,100 @@
         <v>0.996937329007202</v>
       </c>
     </row>
+    <row r="45" spans="1:13">
+      <c r="B45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <v>552</v>
+      </c>
+      <c r="D46" s="17">
+        <f>C46/C48</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>598</v>
+      </c>
+      <c r="D47" s="17">
+        <f>C47/C48</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="B48" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="16">
+        <f>SUM(C47,C46)</f>
+        <v>1150</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1797</v>
+      </c>
+      <c r="D52" s="18">
+        <f>C52/C54</f>
+        <v>0.50041771094402676</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="2">
+        <v>0</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1794</v>
+      </c>
+      <c r="D53" s="18">
+        <f>C53/C54</f>
+        <v>0.49958228905597324</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="16">
+        <f>C52+C53</f>
+        <v>3591</v>
+      </c>
+      <c r="D54" s="2"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H34:M37">
+    <sortCondition descending="1" ref="M34"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>